<commit_message>
Update RSRAFVP Requirements Traceability.xlsx
2021.09.20 update
</commit_message>
<xml_diff>
--- a/doc/reqs/RSRAFVP Requirements Traceability.xlsx
+++ b/doc/reqs/RSRAFVP Requirements Traceability.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ws_gvsu\rsrafvp-app\doc\reqs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFFE0AFC-EF40-4C01-82D3-A86B57AD2958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9581DA10-92D1-4973-AD5C-0292CAD00260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,14 +17,14 @@
     <sheet name="Trace Matrix" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Trace Matrix'!$A$3:$G$76</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Trace Matrix'!$A$3:$H$76</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="183">
   <si>
     <t>Revised Self-Report Assessment of Functional</t>
   </si>
@@ -513,6 +513,80 @@
   </si>
   <si>
     <t>Use case 17</t>
+  </si>
+  <si>
+    <t>Title screen</t>
+  </si>
+  <si>
+    <t>Active Assessment</t>
+  </si>
+  <si>
+    <t>Active Assessment (Reset)</t>
+  </si>
+  <si>
+    <t>View My Assessments</t>
+  </si>
+  <si>
+    <t>S-Assessment</t>
+  </si>
+  <si>
+    <t>Wireframe (screen ref)</t>
+  </si>
+  <si>
+    <t>Q-Assessment</t>
+  </si>
+  <si>
+    <t>App Help</t>
+  </si>
+  <si>
+    <t>USHSS Security</t>
+  </si>
+  <si>
+    <t>USHSS Privacy</t>
+  </si>
+  <si>
+    <t>View All Assessments</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Active Assessment, 
+Q-Assessment, 
+S-Assessment</t>
+  </si>
+  <si>
+    <t>Active Assessment, 
+Q-Assessment</t>
+  </si>
+  <si>
+    <t>Main screen,
+View All Assessments</t>
+  </si>
+  <si>
+    <t>Active Assessment, 
+View My Assessments</t>
+  </si>
+  <si>
+    <t>About, 
+App Help, 
+Answers Help</t>
+  </si>
+  <si>
+    <t>About, 
+App Help, 
+Answers Help, 
+Special Help</t>
+  </si>
+  <si>
+    <t>Login, 
+Main screen, 
+Active Assessment</t>
+  </si>
+  <si>
+    <t>Login, 
+Main screen, 
+View All Assessments</t>
   </si>
 </sst>
 </file>
@@ -617,7 +691,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -676,6 +750,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3951,10 +4028,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3963,19 +4040,20 @@
     <col min="2" max="2" width="20.7109375" style="12" customWidth="1"/>
     <col min="3" max="3" width="81.5703125" style="13" customWidth="1"/>
     <col min="4" max="4" width="32.140625" style="12" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" style="12" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" style="12" customWidth="1"/>
-    <col min="7" max="7" width="25.85546875" style="12" customWidth="1"/>
-    <col min="8" max="16384" width="14.42578125" style="12"/>
+    <col min="5" max="5" width="27" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="12" customWidth="1"/>
+    <col min="8" max="8" width="25.85546875" style="12" customWidth="1"/>
+    <col min="9" max="16384" width="14.42578125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="20.25" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="11"/>
     </row>
-    <row r="3" spans="1:7" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>156</v>
       </c>
@@ -3988,17 +4066,20 @@
       <c r="D3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="F3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="G3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="H3" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="18" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" s="18" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="20">
         <v>0</v>
       </c>
@@ -4011,17 +4092,18 @@
       <c r="D4" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="E4" s="21" t="s">
-        <v>155</v>
-      </c>
+      <c r="E4" s="21"/>
       <c r="F4" s="21" t="s">
         <v>155</v>
       </c>
       <c r="G4" s="21" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="H4" s="21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="17">
         <v>1</v>
       </c>
@@ -4034,8 +4116,9 @@
       <c r="D5" s="19" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="E5" s="22"/>
+    </row>
+    <row r="6" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="17">
         <v>2</v>
       </c>
@@ -4048,8 +4131,9 @@
       <c r="D6" s="19" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="E6" s="22"/>
+    </row>
+    <row r="7" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="17">
         <v>3</v>
       </c>
@@ -4062,8 +4146,9 @@
       <c r="D7" s="19" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E7" s="22"/>
+    </row>
+    <row r="8" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A8" s="17">
         <v>4</v>
       </c>
@@ -4076,8 +4161,11 @@
       <c r="D8" s="19" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="E8" s="22" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A9" s="20">
         <v>5</v>
       </c>
@@ -4090,17 +4178,18 @@
       <c r="D9" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="E9" s="21" t="s">
-        <v>155</v>
-      </c>
+      <c r="E9" s="21"/>
       <c r="F9" s="21" t="s">
         <v>155</v>
       </c>
       <c r="G9" s="21" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="H9" s="21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A10" s="17">
         <v>6</v>
       </c>
@@ -4113,8 +4202,9 @@
       <c r="D10" s="19" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="E10" s="22"/>
+    </row>
+    <row r="11" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="17">
         <v>7</v>
       </c>
@@ -4127,8 +4217,9 @@
       <c r="D11" s="19" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E11" s="22"/>
+    </row>
+    <row r="12" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A12" s="17">
         <v>8</v>
       </c>
@@ -4141,8 +4232,9 @@
       <c r="D12" s="19" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="E12" s="22"/>
+    </row>
+    <row r="13" spans="1:8" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A13" s="17">
         <v>9</v>
       </c>
@@ -4155,8 +4247,11 @@
       <c r="D13" s="19" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="E13" s="22" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A14" s="17">
         <v>10</v>
       </c>
@@ -4169,8 +4264,9 @@
       <c r="D14" s="19" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E14" s="22"/>
+    </row>
+    <row r="15" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A15" s="17">
         <v>11</v>
       </c>
@@ -4183,8 +4279,9 @@
       <c r="D15" s="19" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="E15" s="22"/>
+    </row>
+    <row r="16" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A16" s="17">
         <v>12</v>
       </c>
@@ -4197,8 +4294,11 @@
       <c r="D16" s="17" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E16" s="14" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A17" s="17">
         <v>13</v>
       </c>
@@ -4211,8 +4311,11 @@
       <c r="D17" s="19" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E17" s="22" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A18" s="17">
         <v>14</v>
       </c>
@@ -4225,8 +4328,11 @@
       <c r="D18" s="17" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E18" s="22" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A19" s="17">
         <v>15</v>
       </c>
@@ -4239,8 +4345,11 @@
       <c r="D19" s="17" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E19" s="22" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A20" s="17">
         <v>16</v>
       </c>
@@ -4253,8 +4362,11 @@
       <c r="D20" s="17" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="E20" s="22" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A21" s="17">
         <v>17</v>
       </c>
@@ -4267,8 +4379,11 @@
       <c r="D21" s="17" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="E21" s="14" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A22" s="17">
         <v>18</v>
       </c>
@@ -4281,8 +4396,11 @@
       <c r="D22" s="17" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E22" s="14" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A23" s="17">
         <v>19</v>
       </c>
@@ -4295,8 +4413,11 @@
       <c r="D23" s="17" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E23" s="14" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A24" s="17">
         <v>20</v>
       </c>
@@ -4309,8 +4430,11 @@
       <c r="D24" s="17" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E24" s="14" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A25" s="17">
         <v>21</v>
       </c>
@@ -4323,8 +4447,9 @@
       <c r="D25" s="17" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E25" s="14"/>
+    </row>
+    <row r="26" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A26" s="17">
         <v>22</v>
       </c>
@@ -4337,8 +4462,11 @@
       <c r="D26" s="17" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E26" s="14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A27" s="17">
         <v>23</v>
       </c>
@@ -4351,8 +4479,11 @@
       <c r="D27" s="17" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E27" s="14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A28" s="17">
         <v>24</v>
       </c>
@@ -4365,8 +4496,11 @@
       <c r="D28" s="19" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="E28" s="22" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A29" s="17">
         <v>25</v>
       </c>
@@ -4379,8 +4513,11 @@
       <c r="D29" s="19" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E29" s="22" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A30" s="17">
         <v>26</v>
       </c>
@@ -4393,8 +4530,11 @@
       <c r="D30" s="19" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E30" s="22" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A31" s="17">
         <v>27</v>
       </c>
@@ -4407,8 +4547,11 @@
       <c r="D31" s="17" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="E31" s="14" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A32" s="20">
         <v>28</v>
       </c>
@@ -4421,17 +4564,18 @@
       <c r="D32" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="E32" s="21" t="s">
-        <v>155</v>
-      </c>
+      <c r="E32" s="21"/>
       <c r="F32" s="21" t="s">
         <v>155</v>
       </c>
       <c r="G32" s="21" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="H32" s="21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A33" s="17">
         <v>29</v>
       </c>
@@ -4444,8 +4588,11 @@
       <c r="D33" s="19" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E33" s="22" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A34" s="17">
         <v>30</v>
       </c>
@@ -4458,8 +4605,11 @@
       <c r="D34" s="19" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E34" s="22" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A35" s="17">
         <v>31</v>
       </c>
@@ -4472,8 +4622,11 @@
       <c r="D35" s="19" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E35" s="22" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A36" s="17">
         <v>32</v>
       </c>
@@ -4486,8 +4639,11 @@
       <c r="D36" s="19" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E36" s="22" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A37" s="17">
         <v>33</v>
       </c>
@@ -4500,8 +4656,11 @@
       <c r="D37" s="19" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="E37" s="22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A38" s="17">
         <v>34</v>
       </c>
@@ -4514,8 +4673,11 @@
       <c r="D38" s="19" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="E38" s="22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A39" s="17">
         <v>35</v>
       </c>
@@ -4528,8 +4690,11 @@
       <c r="D39" s="19" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E39" s="22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A40" s="17">
         <v>36</v>
       </c>
@@ -4542,8 +4707,11 @@
       <c r="D40" s="19" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="E40" s="22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A41" s="17">
         <v>37</v>
       </c>
@@ -4556,8 +4724,11 @@
       <c r="D41" s="19" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="E41" s="22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A42" s="17">
         <v>38</v>
       </c>
@@ -4570,8 +4741,11 @@
       <c r="D42" s="19" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="E42" s="22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A43" s="17">
         <v>39</v>
       </c>
@@ -4584,8 +4758,11 @@
       <c r="D43" s="19" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="E43" s="22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A44" s="17">
         <v>40</v>
       </c>
@@ -4598,8 +4775,11 @@
       <c r="D44" s="19" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="E44" s="22" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A45" s="17">
         <v>41</v>
       </c>
@@ -4612,8 +4792,9 @@
       <c r="D45" s="19" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E45" s="22"/>
+    </row>
+    <row r="46" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A46" s="17">
         <v>42</v>
       </c>
@@ -4626,8 +4807,11 @@
       <c r="D46" s="19" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="E46" s="22" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A47" s="20">
         <v>43</v>
       </c>
@@ -4640,17 +4824,18 @@
       <c r="D47" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="E47" s="21" t="s">
-        <v>155</v>
-      </c>
+      <c r="E47" s="21"/>
       <c r="F47" s="21" t="s">
         <v>155</v>
       </c>
       <c r="G47" s="21" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="H47" s="21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A48" s="17">
         <v>44</v>
       </c>
@@ -4663,8 +4848,11 @@
       <c r="D48" s="19" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="E48" s="22" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A49" s="17">
         <v>45</v>
       </c>
@@ -4677,8 +4865,11 @@
       <c r="D49" s="19" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="E49" s="22" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A50" s="17">
         <v>46</v>
       </c>
@@ -4691,8 +4882,11 @@
       <c r="D50" s="19" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="E50" s="22" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A51" s="17">
         <v>47</v>
       </c>
@@ -4705,8 +4899,11 @@
       <c r="D51" s="19" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="E51" s="22" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A52" s="17">
         <v>48</v>
       </c>
@@ -4719,8 +4916,11 @@
       <c r="D52" s="19" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="E52" s="22" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A53" s="17">
         <v>49</v>
       </c>
@@ -4733,8 +4933,11 @@
       <c r="D53" s="19" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E53" s="22" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A54" s="17">
         <v>50</v>
       </c>
@@ -4747,8 +4950,11 @@
       <c r="D54" s="19" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="E54" s="22" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A55" s="20">
         <v>51</v>
       </c>
@@ -4761,17 +4967,18 @@
       <c r="D55" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="E55" s="21" t="s">
-        <v>155</v>
-      </c>
+      <c r="E55" s="21"/>
       <c r="F55" s="21" t="s">
         <v>155</v>
       </c>
       <c r="G55" s="21" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="H55" s="21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A56" s="17">
         <v>52</v>
       </c>
@@ -4784,8 +4991,11 @@
       <c r="D56" s="17" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="E56" s="22" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A57" s="17">
         <v>53</v>
       </c>
@@ -4798,8 +5008,9 @@
       <c r="D57" s="17" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E57" s="14"/>
+    </row>
+    <row r="58" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A58" s="17">
         <v>54</v>
       </c>
@@ -4812,8 +5023,9 @@
       <c r="D58" s="19" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="E58" s="22"/>
+    </row>
+    <row r="59" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A59" s="20">
         <v>55</v>
       </c>
@@ -4826,17 +5038,18 @@
       <c r="D59" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="E59" s="21" t="s">
-        <v>155</v>
-      </c>
+      <c r="E59" s="21"/>
       <c r="F59" s="21" t="s">
         <v>155</v>
       </c>
       <c r="G59" s="21" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="H59" s="21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A60" s="17">
         <v>56</v>
       </c>
@@ -4849,8 +5062,11 @@
       <c r="D60" s="17" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="E60" s="14" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A61" s="17">
         <v>57</v>
       </c>
@@ -4863,8 +5079,11 @@
       <c r="D61" s="17" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E61" s="14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" s="17" customFormat="1" ht="57" x14ac:dyDescent="0.2">
       <c r="A62" s="17">
         <v>58</v>
       </c>
@@ -4877,8 +5096,11 @@
       <c r="D62" s="17" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E62" s="14" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A63" s="17">
         <v>59</v>
       </c>
@@ -4891,8 +5113,11 @@
       <c r="D63" s="17" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E63" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A64" s="17">
         <v>60</v>
       </c>
@@ -4905,8 +5130,11 @@
       <c r="D64" s="17" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="E64" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A65" s="20">
         <v>61</v>
       </c>
@@ -4919,17 +5147,18 @@
       <c r="D65" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="E65" s="21" t="s">
-        <v>155</v>
-      </c>
+      <c r="E65" s="21"/>
       <c r="F65" s="21" t="s">
         <v>155</v>
       </c>
       <c r="G65" s="21" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="H65" s="21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A66" s="17">
         <v>62</v>
       </c>
@@ -4942,8 +5171,11 @@
       <c r="D66" s="17" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E66" s="14" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A67" s="17">
         <v>63</v>
       </c>
@@ -4956,8 +5188,9 @@
       <c r="D67" s="19" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E67" s="22"/>
+    </row>
+    <row r="68" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A68" s="17">
         <v>64</v>
       </c>
@@ -4970,8 +5203,9 @@
       <c r="D68" s="19" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E68" s="22"/>
+    </row>
+    <row r="69" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A69" s="17">
         <v>65</v>
       </c>
@@ -4984,8 +5218,11 @@
       <c r="D69" s="19" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E69" s="22" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A70" s="17">
         <v>66</v>
       </c>
@@ -4998,8 +5235,11 @@
       <c r="D70" s="19" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E70" s="22" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A71" s="17">
         <v>67</v>
       </c>
@@ -5012,8 +5252,11 @@
       <c r="D71" s="17" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E71" s="14" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A72" s="17">
         <v>68</v>
       </c>
@@ -5026,8 +5269,11 @@
       <c r="D72" s="17" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="E72" s="14" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A73" s="20">
         <v>69</v>
       </c>
@@ -5040,17 +5286,18 @@
       <c r="D73" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="E73" s="21" t="s">
-        <v>155</v>
-      </c>
+      <c r="E73" s="21"/>
       <c r="F73" s="21" t="s">
         <v>155</v>
       </c>
       <c r="G73" s="21" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="H73" s="21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A74" s="17">
         <v>70</v>
       </c>
@@ -5063,8 +5310,11 @@
       <c r="D74" s="17" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E74" s="14" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A75" s="17">
         <v>71</v>
       </c>
@@ -5077,8 +5327,11 @@
       <c r="D75" s="17" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E75" s="14" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A76" s="17">
         <v>72</v>
       </c>
@@ -5091,9 +5344,12 @@
       <c r="D76" s="17" t="s">
         <v>157</v>
       </c>
+      <c r="E76" s="14" t="s">
+        <v>174</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:G76" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <autoFilter ref="A3:H76" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Release 1, Version Dec 10, 2021
Updated documentation for Release 1
</commit_message>
<xml_diff>
--- a/doc/reqs/RSRAFVP Requirements Traceability.xlsx
+++ b/doc/reqs/RSRAFVP Requirements Traceability.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ws_gvsu\rsrafvp-app\doc\reqs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9581DA10-92D1-4973-AD5C-0292CAD00260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A9D1CF-0778-4475-AA9A-9D1919EC79D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,14 +17,26 @@
     <sheet name="Trace Matrix" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Trace Matrix'!$A$3:$H$76</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Trace Matrix'!$A$3:$H$77</definedName>
+    <definedName name="_Toc89806513" localSheetId="1">'Trace Matrix'!$H$5</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="220">
   <si>
     <t>Revised Self-Report Assessment of Functional</t>
   </si>
@@ -44,9 +56,6 @@
     <t>Dr. Byron DeVries</t>
   </si>
   <si>
-    <t>CIS Master’s Project, Fall 2021</t>
-  </si>
-  <si>
     <t>Grand Valley State University</t>
   </si>
   <si>
@@ -111,9 +120,6 @@
   </si>
   <si>
     <t xml:space="preserve">The application must be developed using a responsive user interface </t>
-  </si>
-  <si>
-    <t>The application must work on the following browsers</t>
   </si>
   <si>
     <t>The application shall have a splash page which includes the name of the application with version and release date</t>
@@ -587,13 +593,130 @@
     <t>Login, 
 Main screen, 
 View All Assessments</t>
+  </si>
+  <si>
+    <t>The application must work on differet browsers</t>
+  </si>
+  <si>
+    <t>R-SRAFVP Requirements Traceability Matrix</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>inherent in design, no functionality created to allow reassignment of assessments between users</t>
+  </si>
+  <si>
+    <t>inherent in design, no functionality created to allow sharing of assessments between users</t>
+  </si>
+  <si>
+    <t>Deferred to later release</t>
+  </si>
+  <si>
+    <t>CR to remove blank</t>
+  </si>
+  <si>
+    <t>CR to change default to NA</t>
+  </si>
+  <si>
+    <t>Descoped</t>
+  </si>
+  <si>
+    <t>Phone/Tablet/Computer Workflow Scenario</t>
+  </si>
+  <si>
+    <t>If the application has no internet access, the application shall be able to make use of offline functionality</t>
+  </si>
+  <si>
+    <t>Test Case 2</t>
+  </si>
+  <si>
+    <t>Test Case 1, 3</t>
+  </si>
+  <si>
+    <t>Test Case 4, 5</t>
+  </si>
+  <si>
+    <t>Test Case 6, 7, 8, 9, 10, 11, 12</t>
+  </si>
+  <si>
+    <t>Test Case 14</t>
+  </si>
+  <si>
+    <t>Test Case 13, 14</t>
+  </si>
+  <si>
+    <t>Test Case 13, 14, 15</t>
+  </si>
+  <si>
+    <t>Test Case 15</t>
+  </si>
+  <si>
+    <t>Test Case 16</t>
+  </si>
+  <si>
+    <t>Test Case 17</t>
+  </si>
+  <si>
+    <t>Test Case 18</t>
+  </si>
+  <si>
+    <t>Test Case 19</t>
+  </si>
+  <si>
+    <t>Test Case 20</t>
+  </si>
+  <si>
+    <t>Test Case 21</t>
+  </si>
+  <si>
+    <t>Test Case 22, 23</t>
+  </si>
+  <si>
+    <t>Test Case 24</t>
+  </si>
+  <si>
+    <t>Test Case 25, 26</t>
+  </si>
+  <si>
+    <t>Test Case 27</t>
+  </si>
+  <si>
+    <t>Test Case 28</t>
+  </si>
+  <si>
+    <t>Test Case 29</t>
+  </si>
+  <si>
+    <t>Test Case 30</t>
+  </si>
+  <si>
+    <t>Test Case 31</t>
+  </si>
+  <si>
+    <t>Test Case 32</t>
+  </si>
+  <si>
+    <t>Test Case 33</t>
+  </si>
+  <si>
+    <t>Test Case 34</t>
+  </si>
+  <si>
+    <t>CIS693 Final Project, Fall 2021</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Deferred</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -658,8 +781,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -678,6 +807,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -691,7 +826,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -753,6 +888,18 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -976,7 +1123,7 @@
   <dimension ref="A1:A1006"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1037,12 +1184,12 @@
     </row>
     <row r="14" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>6</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
@@ -4028,10 +4175,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H76"/>
+  <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4043,1313 +4190,1990 @@
     <col min="5" max="5" width="27" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.5703125" style="12" customWidth="1"/>
     <col min="7" max="7" width="25.7109375" style="12" customWidth="1"/>
-    <col min="8" max="8" width="25.85546875" style="12" customWidth="1"/>
-    <col min="9" max="16384" width="14.42578125" style="12"/>
+    <col min="8" max="9" width="25.85546875" style="13" customWidth="1"/>
+    <col min="10" max="16384" width="14.42578125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="20.25" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>2</v>
+        <v>182</v>
       </c>
       <c r="C1" s="11"/>
     </row>
-    <row r="3" spans="1:8" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="F3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="F3" s="15" t="s">
+      <c r="G3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="H3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="18" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="I3" s="16" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="18" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="20">
         <v>0</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E4" s="21"/>
       <c r="F4" s="21" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G4" s="21" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+      <c r="I4" s="21"/>
+    </row>
+    <row r="5" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A5" s="17">
         <v>1</v>
       </c>
       <c r="B5" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="I5" s="14"/>
+    </row>
+    <row r="6" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B6" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C6" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="H6" s="24"/>
+      <c r="I6" s="14"/>
+    </row>
+    <row r="7" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="17">
+        <v>2</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D7" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="I7" s="14"/>
+    </row>
+    <row r="8" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="17">
+        <v>3</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="I8" s="14"/>
+    </row>
+    <row r="9" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="17">
+        <v>4</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="I9" s="14"/>
+    </row>
+    <row r="10" spans="1:9" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A10" s="20">
+        <v>5</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="I10" s="21"/>
+    </row>
+    <row r="11" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="17">
+        <v>6</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="I11" s="14"/>
+    </row>
+    <row r="12" spans="1:9" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="17">
+        <v>7</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="H12" s="26"/>
+      <c r="I12" s="14"/>
+    </row>
+    <row r="13" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="17">
+        <v>8</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="H13" s="26"/>
+      <c r="I13" s="14"/>
+    </row>
+    <row r="14" spans="1:9" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="17">
+        <v>9</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="I14" s="14"/>
+    </row>
+    <row r="15" spans="1:9" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A15" s="17">
+        <v>10</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="I15" s="14"/>
+    </row>
+    <row r="16" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="17">
+        <v>11</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="I16" s="14"/>
+    </row>
+    <row r="17" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="17">
+        <v>12</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="I17" s="14"/>
+    </row>
+    <row r="18" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A18" s="17">
+        <v>13</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="H18" s="26"/>
+      <c r="I18" s="14"/>
+    </row>
+    <row r="19" spans="1:9" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="17">
+        <v>14</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="H19" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="I19" s="14"/>
+    </row>
+    <row r="20" spans="1:9" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="17">
+        <v>15</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="H20" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="I20" s="14"/>
+    </row>
+    <row r="21" spans="1:9" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="17">
+        <v>16</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="H21" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="I21" s="14"/>
+    </row>
+    <row r="22" spans="1:9" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="17">
+        <v>17</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="H22" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="I22" s="14"/>
+    </row>
+    <row r="23" spans="1:9" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="17">
+        <v>18</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="H23" s="26"/>
+      <c r="I23" s="14"/>
+    </row>
+    <row r="24" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A24" s="17">
+        <v>19</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A25" s="17">
+        <v>20</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="H25" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="I25" s="14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A26" s="17">
+        <v>21</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="E26" s="14"/>
+      <c r="F26" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="I26" s="14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A27" s="17">
+        <v>22</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="I27" s="14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A28" s="17">
+        <v>23</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="I28" s="14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A29" s="17">
+        <v>24</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="F29" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G29" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="H29" s="26"/>
+      <c r="I29" s="14"/>
+    </row>
+    <row r="30" spans="1:9" s="17" customFormat="1" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A30" s="17">
+        <v>25</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G30" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="H30" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="I30" s="14" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="17" customFormat="1" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A31" s="17">
+        <v>26</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="E31" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="F31" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G31" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="H31" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="I31" s="14" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A32" s="17">
+        <v>27</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G32" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="H32" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="I32" s="14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A33" s="20">
+        <v>28</v>
+      </c>
+      <c r="B33" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="G33" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="H33" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="I33" s="21"/>
+    </row>
+    <row r="34" spans="1:9" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="17">
+        <v>29</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E34" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="G34" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="H34" s="26"/>
+      <c r="I34" s="14"/>
+    </row>
+    <row r="35" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A35" s="17">
+        <v>30</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E35" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="G35" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="H35" s="26"/>
+      <c r="I35" s="14"/>
+    </row>
+    <row r="36" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A36" s="17">
+        <v>31</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="H36" s="26"/>
+      <c r="I36" s="14"/>
+    </row>
+    <row r="37" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A37" s="17">
+        <v>32</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E37" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="G37" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="H37" s="26"/>
+      <c r="I37" s="14"/>
+    </row>
+    <row r="38" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A38" s="17">
+        <v>33</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="F38" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="G38" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="H38" s="26"/>
+      <c r="I38" s="14"/>
+    </row>
+    <row r="39" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A39" s="17">
+        <v>34</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E39" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="F39" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="G39" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="H39" s="26"/>
+      <c r="I39" s="14" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A40" s="17">
+        <v>35</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E40" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="F40" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="H40" s="26"/>
+      <c r="I40" s="14"/>
+    </row>
+    <row r="41" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A41" s="17">
+        <v>36</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E41" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="F41" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="G41" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="H41" s="26"/>
+      <c r="I41" s="14" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A42" s="17">
+        <v>37</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E42" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="F42" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="G42" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="H42" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="I42" s="14" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A43" s="17">
+        <v>38</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E43" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="F43" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="G43" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="H43" s="26"/>
+      <c r="I43" s="14"/>
+    </row>
+    <row r="44" spans="1:9" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A44" s="17">
+        <v>39</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E44" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="F44" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="G44" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="H44" s="26"/>
+      <c r="I44" s="14"/>
+    </row>
+    <row r="45" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A45" s="17">
+        <v>40</v>
+      </c>
+      <c r="B45" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="E45" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="F45" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="G45" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="H45" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="I45" s="14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A46" s="17">
+        <v>41</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D46" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="E5" s="22"/>
-    </row>
-    <row r="6" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="17">
-        <v>2</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="19" t="s">
+      <c r="E46" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F46" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G46" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="H46" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="I46" s="14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A47" s="17">
+        <v>42</v>
+      </c>
+      <c r="B47" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D47" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="17">
-        <v>3</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="19" t="s">
+      <c r="E47" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="F47" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="G47" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="H47" s="26"/>
+      <c r="I47" s="14"/>
+    </row>
+    <row r="48" spans="1:9" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A48" s="20">
+        <v>43</v>
+      </c>
+      <c r="B48" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D48" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="G48" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="H48" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="I48" s="21"/>
+    </row>
+    <row r="49" spans="1:9" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A49" s="17">
+        <v>44</v>
+      </c>
+      <c r="B49" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D49" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E49" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="F49" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="G49" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="H49" s="26"/>
+      <c r="I49" s="14"/>
+    </row>
+    <row r="50" spans="1:9" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A50" s="17">
+        <v>45</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D50" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E50" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="F50" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="G50" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="H50" s="26"/>
+      <c r="I50" s="14"/>
+    </row>
+    <row r="51" spans="1:9" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A51" s="17">
+        <v>46</v>
+      </c>
+      <c r="B51" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D51" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E51" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="F51" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="G51" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="H51" s="26"/>
+      <c r="I51" s="14"/>
+    </row>
+    <row r="52" spans="1:9" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A52" s="17">
+        <v>47</v>
+      </c>
+      <c r="B52" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D52" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E52" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="F52" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="G52" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="H52" s="26"/>
+      <c r="I52" s="14"/>
+    </row>
+    <row r="53" spans="1:9" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A53" s="17">
+        <v>48</v>
+      </c>
+      <c r="B53" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D53" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E53" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="F53" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="G53" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="H53" s="26"/>
+      <c r="I53" s="14"/>
+    </row>
+    <row r="54" spans="1:9" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A54" s="17">
+        <v>49</v>
+      </c>
+      <c r="B54" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D54" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E54" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="F54" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="G54" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="H54" s="26"/>
+      <c r="I54" s="14"/>
+    </row>
+    <row r="55" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A55" s="17">
+        <v>50</v>
+      </c>
+      <c r="B55" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D55" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E55" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="F55" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="G55" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="H55" s="26"/>
+      <c r="I55" s="14"/>
+    </row>
+    <row r="56" spans="1:9" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A56" s="20">
+        <v>51</v>
+      </c>
+      <c r="B56" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="C56" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D56" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="E56" s="21"/>
+      <c r="F56" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="G56" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="H56" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="I56" s="21"/>
+    </row>
+    <row r="57" spans="1:9" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A57" s="17">
+        <v>52</v>
+      </c>
+      <c r="B57" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D57" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="E57" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="F57" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G57" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="H57" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="I57" s="14"/>
+    </row>
+    <row r="58" spans="1:9" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A58" s="17">
+        <v>53</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D58" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="E58" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F58" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G58" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="H58" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="I58" s="14"/>
+    </row>
+    <row r="59" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A59" s="17">
+        <v>54</v>
+      </c>
+      <c r="B59" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D59" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="E59" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F59" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G59" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="H59" s="26"/>
+      <c r="I59" s="14"/>
+    </row>
+    <row r="60" spans="1:9" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A60" s="20">
+        <v>55</v>
+      </c>
+      <c r="B60" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="C60" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D60" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="E60" s="21"/>
+      <c r="F60" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="G60" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="H60" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="I60" s="21"/>
+    </row>
+    <row r="61" spans="1:9" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A61" s="17">
+        <v>56</v>
+      </c>
+      <c r="B61" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="C61" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D61" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="E61" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="F61" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G61" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="H61" s="26"/>
+      <c r="I61" s="14"/>
+    </row>
+    <row r="62" spans="1:9" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A62" s="17">
+        <v>57</v>
+      </c>
+      <c r="B62" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D62" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="8" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="17">
-        <v>4</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="20">
-        <v>5</v>
-      </c>
-      <c r="B9" s="21" t="s">
+      <c r="E62" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="F62" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G62" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="H62" s="26"/>
+      <c r="I62" s="14"/>
+    </row>
+    <row r="63" spans="1:9" s="17" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+      <c r="A63" s="17">
+        <v>58</v>
+      </c>
+      <c r="B63" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D63" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="E63" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="F63" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G63" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="H63" s="26"/>
+      <c r="I63" s="14"/>
+    </row>
+    <row r="64" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A64" s="17">
+        <v>59</v>
+      </c>
+      <c r="B64" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D64" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="E64" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="F64" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G64" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="H64" s="26"/>
+      <c r="I64" s="14"/>
+    </row>
+    <row r="65" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A65" s="17">
+        <v>60</v>
+      </c>
+      <c r="B65" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="D65" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="E65" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="F65" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G65" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="H65" s="26"/>
+      <c r="I65" s="14"/>
+    </row>
+    <row r="66" spans="1:9" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A66" s="20">
+        <v>61</v>
+      </c>
+      <c r="B66" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="C66" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D66" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="E66" s="21"/>
+      <c r="F66" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="G66" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="H66" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="I66" s="21"/>
+    </row>
+    <row r="67" spans="1:9" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A67" s="17">
+        <v>62</v>
+      </c>
+      <c r="B67" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="D67" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="E67" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="F67" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G67" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="H67" s="26"/>
+      <c r="I67" s="14"/>
+    </row>
+    <row r="68" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A68" s="17">
+        <v>63</v>
+      </c>
+      <c r="B68" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="D68" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="E68" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F68" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G68" s="25"/>
+      <c r="H68" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="I68" s="14"/>
+    </row>
+    <row r="69" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A69" s="17">
+        <v>64</v>
+      </c>
+      <c r="B69" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="C69" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="D69" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="E69" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F69" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G69" s="25"/>
+      <c r="H69" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="I69" s="14"/>
+    </row>
+    <row r="70" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A70" s="17">
+        <v>65</v>
+      </c>
+      <c r="B70" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="C70" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D70" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="E70" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="F70" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G70" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="H70" s="26"/>
+      <c r="I70" s="14"/>
+    </row>
+    <row r="71" spans="1:9" s="17" customFormat="1" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A71" s="17">
+        <v>66</v>
+      </c>
+      <c r="B71" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="C71" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D71" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="E71" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="F71" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G71" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="H71" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="I71" s="14" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A72" s="17">
+        <v>67</v>
+      </c>
+      <c r="B72" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C72" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="D72" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="E72" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="F72" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G72" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="H72" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="I72" s="14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A73" s="17">
+        <v>68</v>
+      </c>
+      <c r="B73" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="C73" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="D73" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="E73" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="F73" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G73" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="H73" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="I73" s="14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A74" s="20">
+        <v>69</v>
+      </c>
+      <c r="B74" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="C74" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D74" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="E74" s="21"/>
+      <c r="F74" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="G74" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="H74" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="I74" s="21"/>
+    </row>
+    <row r="75" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A75" s="17">
+        <v>70</v>
+      </c>
+      <c r="B75" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="C75" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="D75" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="E75" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="F75" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="G75" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="H75" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="I75" s="14"/>
+    </row>
+    <row r="76" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A76" s="17">
+        <v>71</v>
+      </c>
+      <c r="B76" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C76" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D76" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="E76" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="F76" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="G76" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="H76" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="I76" s="14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A77" s="17">
+        <v>72</v>
+      </c>
+      <c r="B77" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="C77" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="D77" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="G9" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="H9" s="21" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="17">
-        <v>6</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="E10" s="22"/>
-    </row>
-    <row r="11" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="17">
-        <v>7</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="E11" s="22"/>
-    </row>
-    <row r="12" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="17">
-        <v>8</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="E12" s="22"/>
-    </row>
-    <row r="13" spans="1:8" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="17">
-        <v>9</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="17">
-        <v>10</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="E14" s="22"/>
-    </row>
-    <row r="15" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="17">
-        <v>11</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="E15" s="22"/>
-    </row>
-    <row r="16" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="17">
-        <v>12</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="17">
-        <v>13</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="17">
-        <v>14</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="17">
-        <v>15</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="17">
-        <v>16</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="17">
-        <v>17</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="17">
-        <v>18</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A23" s="17">
-        <v>19</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="17">
-        <v>20</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A25" s="17">
-        <v>21</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>160</v>
-      </c>
-      <c r="E25" s="14"/>
-    </row>
-    <row r="26" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="17">
-        <v>22</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A27" s="17">
-        <v>23</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A28" s="17">
-        <v>24</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="E28" s="22" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A29" s="17">
-        <v>25</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="E29" s="22" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="17">
-        <v>26</v>
-      </c>
-      <c r="B30" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="E30" s="22" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A31" s="17">
-        <v>27</v>
-      </c>
-      <c r="B31" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D31" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="20">
-        <v>28</v>
-      </c>
-      <c r="B32" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="C32" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="D32" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="G32" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="H32" s="21" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="17">
-        <v>29</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="E33" s="22" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A34" s="17">
-        <v>30</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="E34" s="22" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A35" s="17">
-        <v>31</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="C35" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="D35" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="E35" s="22" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A36" s="17">
-        <v>32</v>
-      </c>
-      <c r="B36" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="C36" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="D36" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="E36" s="22" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A37" s="17">
-        <v>33</v>
-      </c>
-      <c r="B37" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="D37" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="E37" s="22" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A38" s="17">
-        <v>34</v>
-      </c>
-      <c r="B38" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="D38" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="E38" s="22" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A39" s="17">
-        <v>35</v>
-      </c>
-      <c r="B39" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="D39" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="E39" s="22" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A40" s="17">
-        <v>36</v>
-      </c>
-      <c r="B40" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="C40" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="D40" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="E40" s="22" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A41" s="17">
-        <v>37</v>
-      </c>
-      <c r="B41" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="C41" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="D41" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="E41" s="22" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A42" s="17">
-        <v>38</v>
-      </c>
-      <c r="B42" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="C42" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="E42" s="22" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A43" s="17">
-        <v>39</v>
-      </c>
-      <c r="B43" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C43" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="D43" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="E43" s="22" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A44" s="17">
-        <v>40</v>
-      </c>
-      <c r="B44" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="C44" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="D44" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="E44" s="22" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A45" s="17">
-        <v>41</v>
-      </c>
-      <c r="B45" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="C45" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="D45" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="E45" s="22"/>
-    </row>
-    <row r="46" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A46" s="17">
-        <v>42</v>
-      </c>
-      <c r="B46" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="C46" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="D46" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="E46" s="22" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A47" s="20">
-        <v>43</v>
-      </c>
-      <c r="B47" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="C47" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="D47" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="E47" s="21"/>
-      <c r="F47" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="G47" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="H47" s="21" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A48" s="17">
-        <v>44</v>
-      </c>
-      <c r="B48" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="C48" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="D48" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="E48" s="22" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A49" s="17">
-        <v>45</v>
-      </c>
-      <c r="B49" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="C49" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="D49" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="E49" s="22" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A50" s="17">
-        <v>46</v>
-      </c>
-      <c r="B50" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="C50" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="D50" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="E50" s="22" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A51" s="17">
-        <v>47</v>
-      </c>
-      <c r="B51" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="C51" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="D51" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="E51" s="22" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A52" s="17">
-        <v>48</v>
-      </c>
-      <c r="B52" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="C52" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="D52" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="E52" s="22" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A53" s="17">
-        <v>49</v>
-      </c>
-      <c r="B53" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="C53" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="D53" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="E53" s="22" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A54" s="17">
-        <v>50</v>
-      </c>
-      <c r="B54" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="C54" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="D54" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="E54" s="22" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A55" s="20">
-        <v>51</v>
-      </c>
-      <c r="B55" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="C55" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="D55" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="E55" s="21"/>
-      <c r="F55" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="G55" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="H55" s="21" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A56" s="17">
-        <v>52</v>
-      </c>
-      <c r="B56" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="C56" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="D56" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="E56" s="22" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A57" s="17">
-        <v>53</v>
-      </c>
-      <c r="B57" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="C57" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="D57" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="E57" s="14"/>
-    </row>
-    <row r="58" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A58" s="17">
-        <v>54</v>
-      </c>
-      <c r="B58" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="C58" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="D58" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="E58" s="22"/>
-    </row>
-    <row r="59" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A59" s="20">
-        <v>55</v>
-      </c>
-      <c r="B59" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="C59" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="D59" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="E59" s="21"/>
-      <c r="F59" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="G59" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="H59" s="21" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A60" s="17">
-        <v>56</v>
-      </c>
-      <c r="B60" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="C60" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="D60" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="E60" s="14" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A61" s="17">
-        <v>57</v>
-      </c>
-      <c r="B61" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="C61" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="D61" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="E61" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" s="17" customFormat="1" ht="57" x14ac:dyDescent="0.2">
-      <c r="A62" s="17">
-        <v>58</v>
-      </c>
-      <c r="B62" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="C62" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="D62" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="E62" s="14" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A63" s="17">
-        <v>59</v>
-      </c>
-      <c r="B63" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="C63" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="D63" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="E63" s="14" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A64" s="17">
-        <v>60</v>
-      </c>
-      <c r="B64" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="C64" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="D64" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="E64" s="14" t="s">
+      <c r="E77" s="14" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A65" s="20">
-        <v>61</v>
-      </c>
-      <c r="B65" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="C65" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="D65" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="E65" s="21"/>
-      <c r="F65" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="G65" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="H65" s="21" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A66" s="17">
-        <v>62</v>
-      </c>
-      <c r="B66" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="C66" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="D66" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="E66" s="14" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A67" s="17">
-        <v>63</v>
-      </c>
-      <c r="B67" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="C67" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="D67" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="E67" s="22"/>
-    </row>
-    <row r="68" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A68" s="17">
-        <v>64</v>
-      </c>
-      <c r="B68" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="C68" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="D68" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="E68" s="22"/>
-    </row>
-    <row r="69" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A69" s="17">
-        <v>65</v>
-      </c>
-      <c r="B69" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="C69" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="D69" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="E69" s="22" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A70" s="17">
-        <v>66</v>
-      </c>
-      <c r="B70" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="C70" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="D70" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="E70" s="22" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A71" s="17">
-        <v>67</v>
-      </c>
-      <c r="B71" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="C71" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="D71" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="E71" s="14" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" s="17" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A72" s="17">
-        <v>68</v>
-      </c>
-      <c r="B72" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="C72" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="D72" s="17" t="s">
-        <v>160</v>
-      </c>
-      <c r="E72" s="14" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A73" s="20">
-        <v>69</v>
-      </c>
-      <c r="B73" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="C73" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="D73" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="E73" s="21"/>
-      <c r="F73" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="G73" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="H73" s="21" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A74" s="17">
-        <v>70</v>
-      </c>
-      <c r="B74" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="C74" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D74" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="E74" s="14" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A75" s="17">
-        <v>71</v>
-      </c>
-      <c r="B75" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="C75" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="D75" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="E75" s="14" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" s="17" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A76" s="17">
-        <v>72</v>
-      </c>
-      <c r="B76" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="C76" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="D76" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="E76" s="14" t="s">
-        <v>174</v>
-      </c>
+      <c r="F77" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="G77" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="H77" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="I77" s="14"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:H76" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <autoFilter ref="A3:H77" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>